<commit_message>
adicion documentacion y cliente
</commit_message>
<xml_diff>
--- a/documentation/00. General/Cronograma de Actividades.xlsx
+++ b/documentation/00. General/Cronograma de Actividades.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JS22\Recursos\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JS22\WorkSpace\ProyectoFacturador\documentation\00. General\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE771708-8FFC-4351-8698-C450599472C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36C2E39F-6989-49DB-8B14-6C042DC256EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0D86061E-64ED-4CC1-A86A-AA6D3E8E114A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Tarea</t>
   </si>
@@ -92,13 +92,7 @@
     <t>Desarrollo de Interfaz de usuario (FrontEnd)</t>
   </si>
   <si>
-    <t>En Progreso</t>
-  </si>
-  <si>
     <t>Ejecutar pruebas de Aseguramiento de Calidad</t>
-  </si>
-  <si>
-    <t>Por Hacer</t>
   </si>
   <si>
     <t>Completar Desarrollos</t>
@@ -129,7 +123,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,24 +170,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFED7D31"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,12 +205,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -313,12 +285,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -326,9 +292,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -337,12 +300,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -352,23 +315,20 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -687,7 +647,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,102 +662,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32" t="s">
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="33">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="17">
         <v>1</v>
       </c>
-      <c r="H2" s="34">
+      <c r="H2" s="18">
         <v>2</v>
       </c>
-      <c r="I2" s="34">
+      <c r="I2" s="18">
         <v>3</v>
       </c>
-      <c r="J2" s="34">
+      <c r="J2" s="18">
         <v>4</v>
       </c>
-      <c r="K2" s="33">
+      <c r="K2" s="17">
         <v>1</v>
       </c>
-      <c r="L2" s="34">
+      <c r="L2" s="18">
         <v>2</v>
       </c>
-      <c r="M2" s="34">
+      <c r="M2" s="18">
         <v>3</v>
       </c>
-      <c r="N2" s="34">
+      <c r="N2" s="18">
         <v>4</v>
       </c>
-      <c r="O2" s="33">
+      <c r="O2" s="17">
         <v>1</v>
       </c>
-      <c r="P2" s="34">
+      <c r="P2" s="18">
         <v>2</v>
       </c>
-      <c r="Q2" s="34">
+      <c r="Q2" s="18">
         <v>3</v>
       </c>
-      <c r="R2" s="34">
+      <c r="R2" s="18">
         <v>4</v>
       </c>
-      <c r="S2" s="33">
+      <c r="S2" s="17">
         <v>1</v>
       </c>
-      <c r="T2" s="34">
+      <c r="T2" s="18">
         <v>2</v>
       </c>
-      <c r="U2" s="34">
+      <c r="U2" s="18">
         <v>3</v>
       </c>
-      <c r="V2" s="34">
+      <c r="V2" s="18">
         <v>4</v>
       </c>
     </row>
@@ -810,24 +770,24 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
-      <c r="V3" s="31"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="21"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -848,22 +808,22 @@
       <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="16"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="13"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -884,22 +844,22 @@
       <c r="F5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="16"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="13"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -910,24 +870,24 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="31"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="21"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -948,22 +908,22 @@
       <c r="F7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="16"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="13"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -984,22 +944,22 @@
       <c r="F8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="16"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="13"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1010,24 +970,24 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="31"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="21"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -1048,22 +1008,22 @@
       <c r="F10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="16"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="13"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1084,22 +1044,22 @@
       <c r="F11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="16"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="13"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1120,22 +1080,22 @@
       <c r="F12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="16"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="13"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1153,57 +1113,57 @@
       <c r="E13" s="4">
         <v>25</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="16"/>
+      <c r="F13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="13"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="30"/>
-      <c r="U14" s="30"/>
-      <c r="V14" s="31"/>
+      <c r="G14" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="21"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>8</v>
@@ -1217,29 +1177,29 @@
       <c r="E15" s="4">
         <v>8</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="16"/>
+      <c r="F15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="13"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>8</v>
@@ -1253,65 +1213,60 @@
       <c r="E16" s="4">
         <v>3</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="13"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="25"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="16"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12">
+      <c r="B17" s="9"/>
+      <c r="C17" s="10">
         <v>44179</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="10">
         <v>44179</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="U17" s="27"/>
-      <c r="V17" s="28"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="G3:V3"/>
-    <mergeCell ref="G6:V6"/>
-    <mergeCell ref="G9:V9"/>
-    <mergeCell ref="G17:V17"/>
-    <mergeCell ref="G14:V14"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="O1:R1"/>
@@ -1322,6 +1277,11 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G3:V3"/>
+    <mergeCell ref="G6:V6"/>
+    <mergeCell ref="G9:V9"/>
+    <mergeCell ref="G17:V17"/>
+    <mergeCell ref="G14:V14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>